<commit_message>
CTMS: Add site test case - fixes
</commit_message>
<xml_diff>
--- a/src/test/resources/data/DESKTOP_WEB/SiteManagement/SiteManagementTestData.xlsx
+++ b/src/test/resources/data/DESKTOP_WEB/SiteManagement/SiteManagementTestData.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Password</t>
   </si>
@@ -34,6 +34,18 @@
   </si>
   <si>
     <t>AddNewSite</t>
+  </si>
+  <si>
+    <t>Study Phase</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Phase II/III</t>
+  </si>
+  <si>
+    <t>Planning</t>
   </si>
 </sst>
 </file>
@@ -363,7 +375,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -396,8 +408,12 @@
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
+      <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="2" spans="1:5">
       <c r="B2" s="2" t="s">
@@ -405,6 +421,12 @@
       </c>
       <c r="C2" s="2" t="s">
         <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:5">

</xml_diff>

<commit_message>
CTMS: Added visit schedule test case
</commit_message>
<xml_diff>
--- a/src/test/resources/data/DESKTOP_WEB/SiteManagement/SiteManagementTestData.xlsx
+++ b/src/test/resources/data/DESKTOP_WEB/SiteManagement/SiteManagementTestData.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="12">
   <si>
     <t>Password</t>
   </si>
@@ -46,6 +46,15 @@
   </si>
   <si>
     <t>Planning</t>
+  </si>
+  <si>
+    <t>AddVisitScheduleForSite</t>
+  </si>
+  <si>
+    <t>Qualification Visit</t>
+  </si>
+  <si>
+    <t>Category</t>
   </si>
 </sst>
 </file>
@@ -375,7 +384,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -383,10 +392,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:E2"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -398,7 +407,7 @@
     <col min="5" max="5" width="6.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -415,7 +424,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:6">
       <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
@@ -429,12 +438,44 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="5" spans="1:6">
+      <c r="B5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
     </row>

</xml_diff>

<commit_message>
CTMS: Added test step - assigned questionnaire
</commit_message>
<xml_diff>
--- a/src/test/resources/data/DESKTOP_WEB/SiteManagement/SiteManagementTestData.xlsx
+++ b/src/test/resources/data/DESKTOP_WEB/SiteManagement/SiteManagementTestData.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="16">
   <si>
     <t>Password</t>
   </si>
@@ -55,6 +55,18 @@
   </si>
   <si>
     <t>Category</t>
+  </si>
+  <si>
+    <t>QuestionnaireAssignedTo</t>
+  </si>
+  <si>
+    <t>Study</t>
+  </si>
+  <si>
+    <t>Template Name</t>
+  </si>
+  <si>
+    <t>SQV Report</t>
   </si>
 </sst>
 </file>
@@ -384,7 +396,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -392,10 +404,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -407,7 +419,7 @@
     <col min="5" max="5" width="6.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -424,7 +436,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:8">
       <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
@@ -438,7 +450,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -457,8 +469,14 @@
       <c r="F4" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="G4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:8">
       <c r="B5" s="2" t="s">
         <v>1</v>
       </c>
@@ -474,8 +492,14 @@
       <c r="F5" t="s">
         <v>10</v>
       </c>
+      <c r="G5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H5" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:8">
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
     </row>

</xml_diff>

<commit_message>
CTMS: Added template step to sites test case
</commit_message>
<xml_diff>
--- a/src/test/resources/data/DESKTOP_WEB/SiteManagement/SiteManagementTestData.xlsx
+++ b/src/test/resources/data/DESKTOP_WEB/SiteManagement/SiteManagementTestData.xlsx
@@ -48,9 +48,6 @@
     <t>Planning</t>
   </si>
   <si>
-    <t>AddVisitScheduleForSite</t>
-  </si>
-  <si>
     <t>Qualification Visit</t>
   </si>
   <si>
@@ -67,6 +64,9 @@
   </si>
   <si>
     <t>SQV Report</t>
+  </si>
+  <si>
+    <t>AddVisitReportAndScheduleForSite</t>
   </si>
 </sst>
 </file>
@@ -396,7 +396,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -407,7 +407,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -452,7 +452,7 @@
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>3</v>
@@ -467,13 +467,13 @@
         <v>6</v>
       </c>
       <c r="F4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="H4" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -490,13 +490,13 @@
         <v>8</v>
       </c>
       <c r="F5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:8">

</xml_diff>

<commit_message>
CTMS: ViewReport e2e flow complete
</commit_message>
<xml_diff>
--- a/src/test/resources/data/DESKTOP_WEB/SiteManagement/SiteManagementTestData.xlsx
+++ b/src/test/resources/data/DESKTOP_WEB/SiteManagement/SiteManagementTestData.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="18">
   <si>
     <t>Password</t>
   </si>
@@ -67,6 +67,12 @@
   </si>
   <si>
     <t>AddVisitReportAndScheduleForSite</t>
+  </si>
+  <si>
+    <t>ReportStatus</t>
+  </si>
+  <si>
+    <t>Authoring (Default)</t>
   </si>
 </sst>
 </file>
@@ -404,10 +410,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -419,7 +425,7 @@
     <col min="5" max="5" width="6.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -436,7 +442,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:9">
       <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
@@ -450,7 +456,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -475,8 +481,11 @@
       <c r="H4" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="I4" s="1" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:9">
       <c r="B5" s="2" t="s">
         <v>1</v>
       </c>
@@ -498,8 +507,11 @@
       <c r="H5" t="s">
         <v>14</v>
       </c>
+      <c r="I5" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:9">
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
     </row>

</xml_diff>

<commit_message>
CTMS: Added a sample test case which will fail, for reporting purpose.
</commit_message>
<xml_diff>
--- a/src/test/resources/data/DESKTOP_WEB/SiteManagement/SiteManagementTestData.xlsx
+++ b/src/test/resources/data/DESKTOP_WEB/SiteManagement/SiteManagementTestData.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="22">
   <si>
     <t>Password</t>
   </si>
@@ -73,6 +73,18 @@
   </si>
   <si>
     <t>Authoring (Default)</t>
+  </si>
+  <si>
+    <t>SuccessMsgMasterTmplCreation</t>
+  </si>
+  <si>
+    <t>Successfully created 1 records</t>
+  </si>
+  <si>
+    <t>SuccessMsg</t>
+  </si>
+  <si>
+    <t>1 record(s) successfully entered.</t>
   </si>
 </sst>
 </file>
@@ -402,7 +414,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -410,10 +422,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -425,7 +437,7 @@
     <col min="5" max="5" width="6.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -441,8 +453,11 @@
       <c r="E1" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="F1" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:11">
       <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
@@ -455,8 +470,11 @@
       <c r="E2" t="s">
         <v>8</v>
       </c>
+      <c r="F2" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:11">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -484,8 +502,14 @@
       <c r="I4" s="1" t="s">
         <v>16</v>
       </c>
+      <c r="J4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:11">
       <c r="B5" s="2" t="s">
         <v>1</v>
       </c>
@@ -510,8 +534,14 @@
       <c r="I5" t="s">
         <v>17</v>
       </c>
+      <c r="J5" t="s">
+        <v>19</v>
+      </c>
+      <c r="K5" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:11">
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
     </row>

</xml_diff>

<commit_message>
CTMS: Added eSign CRA Submission step
</commit_message>
<xml_diff>
--- a/src/test/resources/data/DESKTOP_WEB/SiteManagement/SiteManagementTestData.xlsx
+++ b/src/test/resources/data/DESKTOP_WEB/SiteManagement/SiteManagementTestData.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="26">
   <si>
     <t>Password</t>
   </si>
@@ -69,9 +69,6 @@
     <t>AddVisitReportAndScheduleForSite</t>
   </si>
   <si>
-    <t>ReportStatus</t>
-  </si>
-  <si>
     <t>Authoring (Default)</t>
   </si>
   <si>
@@ -81,10 +78,25 @@
     <t>Successfully created 1 records</t>
   </si>
   <si>
-    <t>SuccessMsg</t>
-  </si>
-  <si>
     <t>1 record(s) successfully entered.</t>
+  </si>
+  <si>
+    <t>CRA Submission</t>
+  </si>
+  <si>
+    <t>anuragk</t>
+  </si>
+  <si>
+    <t>Password1</t>
+  </si>
+  <si>
+    <t>ReportStatusBeforeUpdate</t>
+  </si>
+  <si>
+    <t>ReportStatusAfterUpdate</t>
+  </si>
+  <si>
+    <t>SuccessMsgForRecordCreation</t>
   </si>
 </sst>
 </file>
@@ -422,22 +434,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:P7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="44.109375" customWidth="1"/>
-    <col min="2" max="2" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.44140625" customWidth="1"/>
+    <col min="1" max="1" width="29.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.77734375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="27.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:16">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -454,10 +473,10 @@
         <v>6</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:16">
       <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
@@ -471,10 +490,10 @@
         <v>8</v>
       </c>
       <c r="F2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:16">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -500,21 +519,28 @@
         <v>13</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>20</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:16">
       <c r="B5" s="2" t="s">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="D5" t="s">
         <v>7</v>
@@ -532,16 +558,19 @@
         <v>14</v>
       </c>
       <c r="I5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J5" t="s">
+        <v>18</v>
+      </c>
+      <c r="K5" t="s">
         <v>19</v>
       </c>
-      <c r="K5" t="s">
-        <v>21</v>
+      <c r="L5" t="s">
+        <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:16">
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
     </row>

</xml_diff>